<commit_message>
tiendita en excel continuacion
</commit_message>
<xml_diff>
--- a/1120-OpenPyXL/productos.xlsx
+++ b/1120-OpenPyXL/productos.xlsx
@@ -68,7 +68,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -445,107 +448,124 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.4375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="13.8" customHeight="1" s="2">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>producto</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>precio</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>cantidad</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.8" customHeight="1" s="1">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="13.8" customHeight="1" s="2">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>platanitos</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="1">
-      <c r="A3" s="2" t="inlineStr">
+    <row r="3" ht="13.8" customHeight="1" s="2">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>sabritones</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="1">
-      <c r="A4" s="2" t="inlineStr">
+    <row r="4" ht="13.8" customHeight="1" s="2">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>tortillas</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="13.8" customHeight="1" s="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>cocas</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" ht="13.8" customHeight="1" s="1">
-      <c r="A6" s="2" t="inlineStr">
+    <row r="5" ht="13.8" customHeight="1" s="2">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>borrado</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>borrado</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>borrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="13.8" customHeight="1" s="2">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>frutas</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>5.5</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="13.8" customHeight="1" s="1">
-      <c r="A7" s="2" t="inlineStr">
+    <row r="7" ht="13.8" customHeight="1" s="2">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Doritos</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="2">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>roles de canela</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>